<commit_message>
Changed Categorization of Synopsys from Manufacturing Equipment to IP Holder
</commit_message>
<xml_diff>
--- a/manually_edited_data/interest_groups_categories_result.xlsx
+++ b/manually_edited_data/interest_groups_categories_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Python Data Science\Transparency Project\manually_edited_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58F374D-C161-4B6B-8F2D-B55074F85B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227F1A0C-7129-4420-A57A-37B01DFCCA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,7 +505,7 @@
     <t>Synopsys Inc.</t>
   </si>
   <si>
-    <t>Manufacturing Equipment &amp; Design Software</t>
+    <t>Manufacturing Equipment</t>
   </si>
 </sst>
 </file>
@@ -579,55 +579,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
@@ -669,6 +620,55 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -683,10 +683,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F6E6A0F5-F88B-43A9-88BD-865EC7D29602}" name="Tabelle4" displayName="Tabelle4" ref="A1:E57" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F6E6A0F5-F88B-43A9-88BD-865EC7D29602}" name="Tabelle4" displayName="Tabelle4" ref="A1:E57" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:E57" xr:uid="{F6E6A0F5-F88B-43A9-88BD-865EC7D29602}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E57">
-    <sortCondition ref="B1:B57"/>
+    <sortCondition ref="D1:D57"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{61215928-CE51-431A-A778-94C7C8DEB04C}" name="Transparency register ID"/>
@@ -704,7 +704,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15D2E3B7-45C0-4D01-96A7-86D225A2871C}" name="Tabelle1" displayName="Tabelle1" ref="A1:E51" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15D2E3B7-45C0-4D01-96A7-86D225A2871C}" name="Tabelle1" displayName="Tabelle1" ref="A1:E51" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:E51" xr:uid="{15D2E3B7-45C0-4D01-96A7-86D225A2871C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E51">
     <sortCondition ref="D1:D51"/>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042D5856-877B-46DD-8012-CF8B8AB8466A}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1093,54 +1093,58 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C4" t="str">
         <f>_xlfn.XLOOKUP(A4,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.XLOOKUP($A4,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>Fabless (Chip Design &amp; IP Holders)</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" t="s">
-        <v>156</v>
+        <v>15</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xlfn.XLOOKUP(A5,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
+        <v>Semiconductor Industry</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xlfn.XLOOKUP($A5,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
+        <v>Fabless (Chip Design &amp; IP Holders)</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" t="s">
-        <v>141</v>
+        <v>55</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xlfn.XLOOKUP(A6,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
+        <v>Semiconductor Industry</v>
+      </c>
+      <c r="D6" t="str">
+        <f>_xlfn.XLOOKUP($A6,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
+        <v>Fabless (Chip Design &amp; IP Holders)</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.XLOOKUP(A7,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1153,10 +1157,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.XLOOKUP(A8,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1164,205 +1168,201 @@
       </c>
       <c r="D8" t="str">
         <f>_xlfn.XLOOKUP($A8,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Manufacturing Equipment &amp; Design Software</v>
+        <v>Fabless (Chip Design &amp; IP Holders)</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" t="s">
-        <v>143</v>
+        <v>83</v>
+      </c>
+      <c r="C9" t="str">
+        <f>_xlfn.XLOOKUP(A9,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
+        <v>Semiconductor Industry</v>
+      </c>
+      <c r="D9" t="str">
+        <f>_xlfn.XLOOKUP($A9,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
+        <v>Fabless (Chip Design &amp; IP Holders)</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="str">
-        <f>_xlfn.XLOOKUP(A10,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
-      </c>
-      <c r="D10" t="str">
-        <f>_xlfn.XLOOKUP($A10,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Foundry</v>
+        <v>148</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.XLOOKUP(A11,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D11" t="str">
         <f>_xlfn.XLOOKUP($A11,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>Fabless (Chip Design &amp; IP Holders)</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.XLOOKUP(A12,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Thinktank</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D12" t="str">
         <f>_xlfn.XLOOKUP($A12,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Thinktank</v>
+        <v>Fabless (Chip Design &amp; IP Holders)</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.XLOOKUP(A13,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Thinktank</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D13" t="str">
         <f>_xlfn.XLOOKUP($A13,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Thinktank</v>
+        <v>Fabless (Chip Design &amp; IP Holders)</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="str">
-        <f>_xlfn.XLOOKUP(A14,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
-      </c>
-      <c r="D14" t="str">
-        <f>_xlfn.XLOOKUP($A14,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Fabless (Chip Design &amp; IP Holders)</v>
+        <v>155</v>
+      </c>
+      <c r="C14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.XLOOKUP(A15,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Research and Development</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D15" t="str">
         <f>_xlfn.XLOOKUP($A15,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Research and Development</v>
+        <v>Fabless (Chip Design &amp; IP Holders)</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.XLOOKUP(A16,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D16" t="str">
         <f>_xlfn.XLOOKUP($A16,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>Foundry</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.XLOOKUP(A17,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D17" t="str">
         <f>_xlfn.XLOOKUP($A17,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>Foundry</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="C18" t="str">
         <f>_xlfn.XLOOKUP(A18,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D18" t="str">
         <f>_xlfn.XLOOKUP($A18,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>Foundry</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.XLOOKUP(A19,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D19" t="str">
         <f>_xlfn.XLOOKUP($A19,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>Foundry</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="str">
-        <f>_xlfn.XLOOKUP(A20,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
-      </c>
-      <c r="D20" t="str">
-        <f>_xlfn.XLOOKUP($A20,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.XLOOKUP(A21,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1375,26 +1375,24 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>151</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" t="str">
-        <f>_xlfn.XLOOKUP(A22,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
-      </c>
-      <c r="D22" t="str">
-        <f>_xlfn.XLOOKUP($A22,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>152</v>
+      </c>
+      <c r="C22" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.XLOOKUP(A23,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1407,10 +1405,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C24" t="str">
         <f>_xlfn.XLOOKUP(A24,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1423,74 +1421,74 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.XLOOKUP(A25,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Research and Development</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D25" t="str">
         <f>_xlfn.XLOOKUP($A25,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Research and Development</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C26" t="str">
         <f>_xlfn.XLOOKUP(A26,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Research and Development</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D26" t="str">
         <f>_xlfn.XLOOKUP($A26,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Research and Development</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C27" t="str">
         <f>_xlfn.XLOOKUP(A27,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D27" t="str">
         <f>_xlfn.XLOOKUP($A27,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Foundry</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.XLOOKUP(A28,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D28" t="str">
         <f>_xlfn.XLOOKUP($A28,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Fabless (Chip Design &amp; IP Holders)</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.XLOOKUP(A29,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1503,120 +1501,122 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="C30" t="str">
         <f>_xlfn.XLOOKUP(A30,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D30" t="str">
         <f>_xlfn.XLOOKUP($A30,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Integrated Device Manufacturer (IDM)</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C31" t="str">
         <f>_xlfn.XLOOKUP(A31,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D31" t="str">
         <f>_xlfn.XLOOKUP($A31,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Integrated Device Manufacturer (IDM)</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.XLOOKUP(A32,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Research and Development</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D32" t="str">
         <f>_xlfn.XLOOKUP($A32,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Research and Development</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="C33" t="str">
         <f>_xlfn.XLOOKUP(A33,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D33" t="str">
         <f>_xlfn.XLOOKUP($A33,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Fabless (Chip Design &amp; IP Holders)</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C34" t="str">
         <f>_xlfn.XLOOKUP(A34,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D34" t="str">
         <f>_xlfn.XLOOKUP($A34,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Fabless (Chip Design &amp; IP Holders)</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C35" t="str">
         <f>_xlfn.XLOOKUP(A35,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Industry stakeholder</v>
       </c>
       <c r="D35" t="str">
         <f>_xlfn.XLOOKUP($A35,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Fabless (Chip Design &amp; IP Holders)</v>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" t="s">
-        <v>144</v>
+        <v>25</v>
+      </c>
+      <c r="C36" t="str">
+        <f>_xlfn.XLOOKUP(A36,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
+        <v>Industry stakeholder</v>
+      </c>
+      <c r="D36" t="str">
+        <f>_xlfn.XLOOKUP($A36,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
+        <v>Industry stakeholder</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C37" t="str">
         <f>_xlfn.XLOOKUP(A37,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1629,26 +1629,26 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="C38" t="str">
         <f>_xlfn.XLOOKUP(A38,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D38" t="str">
         <f>_xlfn.XLOOKUP($A38,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>Integrated Device Manufacturer (IDM)</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C39" t="str">
         <f>_xlfn.XLOOKUP(A39,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1656,15 +1656,15 @@
       </c>
       <c r="D39" t="str">
         <f>_xlfn.XLOOKUP($A39,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Fabless (Chip Design &amp; IP Holders)</v>
+        <v>Integrated Device Manufacturer (IDM)</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C40" t="str">
         <f>_xlfn.XLOOKUP(A40,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1672,47 +1672,45 @@
       </c>
       <c r="D40" t="str">
         <f>_xlfn.XLOOKUP($A40,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Fabless (Chip Design &amp; IP Holders)</v>
+        <v>Integrated Device Manufacturer (IDM)</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" t="str">
-        <f>_xlfn.XLOOKUP(A41,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
-      </c>
-      <c r="D41" t="str">
-        <f>_xlfn.XLOOKUP($A41,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Fabless (Chip Design &amp; IP Holders)</v>
+        <v>146</v>
+      </c>
+      <c r="C41" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="C42" t="str">
         <f>_xlfn.XLOOKUP(A42,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Non Semiconductor Industry</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D42" t="str">
         <f>_xlfn.XLOOKUP($A42,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Non Semiconductor Industry: Other</v>
+        <v>Manufacturing Equipment</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="C43" t="str">
         <f>_xlfn.XLOOKUP(A43,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
@@ -1720,227 +1718,229 @@
       </c>
       <c r="D43" t="str">
         <f>_xlfn.XLOOKUP($A43,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Integrated Device Manufacturer (IDM)</v>
+        <v>Manufacturing Equipment</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="C44" t="str">
         <f>_xlfn.XLOOKUP(A44,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Non Semiconductor Industry</v>
+        <v>Semiconductor Industry</v>
       </c>
       <c r="D44" t="str">
         <f>_xlfn.XLOOKUP($A44,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Non Semiconductor Industry: Automotive</v>
+        <v>Manufacturing Equipment</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="C45" t="str">
         <f>_xlfn.XLOOKUP(A45,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
+        <v>Non Semiconductor Industry</v>
       </c>
       <c r="D45" t="str">
         <f>_xlfn.XLOOKUP($A45,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>Non Semiconductor Industry: Automotive</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="C46" t="str">
         <f>_xlfn.XLOOKUP(A46,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Non Semiconductor Industry</v>
       </c>
       <c r="D46" t="str">
         <f>_xlfn.XLOOKUP($A46,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Manufacturing Equipment &amp; Design Software</v>
+        <v>Non Semiconductor Industry: Automotive</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C47" t="str">
         <f>_xlfn.XLOOKUP(A47,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Non Semiconductor Industry</v>
       </c>
       <c r="D47" t="str">
         <f>_xlfn.XLOOKUP($A47,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Manufacturing Equipment &amp; Design Software</v>
+        <v>Non Semiconductor Industry: Automotive</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" t="str">
-        <f>_xlfn.XLOOKUP(A48,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Non Semiconductor Industry</v>
-      </c>
-      <c r="D48" t="str">
-        <f>_xlfn.XLOOKUP($A48,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Non Semiconductor Industry: Automotive</v>
+        <v>150</v>
+      </c>
+      <c r="C48" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="C49" t="str">
         <f>_xlfn.XLOOKUP(A49,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Thinktank</v>
+        <v>Non Semiconductor Industry</v>
       </c>
       <c r="D49" t="str">
         <f>_xlfn.XLOOKUP($A49,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Thinktank</v>
+        <v>Non Semiconductor Industry: Other</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C50" t="str">
         <f>_xlfn.XLOOKUP(A50,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Non Semiconductor Industry</v>
       </c>
       <c r="D50" t="str">
         <f>_xlfn.XLOOKUP($A50,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Foundry</v>
+        <v>Non Semiconductor Industry: Other</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
-      </c>
-      <c r="C51" t="s">
-        <v>134</v>
-      </c>
-      <c r="D51" t="s">
-        <v>156</v>
+        <v>95</v>
+      </c>
+      <c r="C51" t="str">
+        <f>_xlfn.XLOOKUP(A51,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
+        <v>Research and Development</v>
+      </c>
+      <c r="D51" t="str">
+        <f>_xlfn.XLOOKUP($A51,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
+        <v>Research and Development</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C52" t="str">
         <f>_xlfn.XLOOKUP(A52,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Research and Development</v>
       </c>
       <c r="D52" t="str">
         <f>_xlfn.XLOOKUP($A52,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Foundry</v>
+        <v>Research and Development</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" t="s">
-        <v>134</v>
-      </c>
-      <c r="D53" t="s">
-        <v>104</v>
+        <v>47</v>
+      </c>
+      <c r="C53" t="str">
+        <f>_xlfn.XLOOKUP(A53,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
+        <v>Research and Development</v>
+      </c>
+      <c r="D53" t="str">
+        <f>_xlfn.XLOOKUP($A53,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
+        <v>Research and Development</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C54" t="str">
         <f>_xlfn.XLOOKUP(A54,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Semiconductor Industry</v>
+        <v>Research and Development</v>
       </c>
       <c r="D54" t="str">
         <f>_xlfn.XLOOKUP($A54,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Fabless (Chip Design &amp; IP Holders)</v>
+        <v>Research and Development</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C55" t="str">
         <f>_xlfn.XLOOKUP(A55,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Non Semiconductor Industry</v>
+        <v>Thinktank</v>
       </c>
       <c r="D55" t="str">
         <f>_xlfn.XLOOKUP($A55,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Non Semiconductor Industry: Other</v>
+        <v>Thinktank</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="C56" t="str">
         <f>_xlfn.XLOOKUP(A56,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Industry stakeholder</v>
+        <v>Thinktank</v>
       </c>
       <c r="D56" t="str">
         <f>_xlfn.XLOOKUP($A56,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Industry stakeholder</v>
+        <v>Thinktank</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C57" t="str">
         <f>_xlfn.XLOOKUP(A57,data_old!$A$2:$A$58,data_old!C$2:C$58,)</f>
-        <v>Non Semiconductor Industry</v>
+        <v>Thinktank</v>
       </c>
       <c r="D57" t="str">
         <f>_xlfn.XLOOKUP($A57,data_old!$A$2:$A$58,data_old!D$2:D$58)</f>
-        <v>Non Semiconductor Industry: Automotive</v>
+        <v>Thinktank</v>
       </c>
     </row>
   </sheetData>
@@ -1956,7 +1956,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45:C48"/>
+      <selection activeCell="D37" sqref="D37:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2796,7 +2796,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>